<commit_message>
Add keeper selections to workbook
</commit_message>
<xml_diff>
--- a/files/keepers18-19.xlsx
+++ b/files/keepers18-19.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="0" windowWidth="19485" windowHeight="5010" activeTab="2"/>
+    <workbookView xWindow="30" yWindow="0" windowWidth="19485" windowHeight="5010"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="11" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1564" uniqueCount="386">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1666" uniqueCount="387">
   <si>
     <t>Ryan Miller</t>
   </si>
@@ -1180,6 +1180,9 @@
   </si>
   <si>
     <t>Enter your team name here</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -2048,9 +2051,7 @@
   </sheetPr>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2077,15 +2078,15 @@
       </c>
       <c r="B2">
         <f>COUNTIFS('Selected keepers'!B:B,A2,'Selected keepers'!E:E,"x")</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C2">
         <f>SUMIFS('Selected keepers'!J:J,'Selected keepers'!B:B,A2,'Selected keepers'!E:E,"x")</f>
-        <v>0</v>
+        <v>5171</v>
       </c>
       <c r="D2">
         <f>'Team salary worksheet'!$N$11-C2</f>
-        <v>6180</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -2094,15 +2095,15 @@
       </c>
       <c r="B3">
         <f>COUNTIFS('Selected keepers'!B:B,A3,'Selected keepers'!E:E,"x")</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="C3">
         <f>SUMIFS('Selected keepers'!J:J,'Selected keepers'!B:B,A3,'Selected keepers'!E:E,"x")</f>
-        <v>0</v>
+        <v>5995</v>
       </c>
       <c r="D3">
         <f>'Team salary worksheet'!$N$11-C3</f>
-        <v>6180</v>
+        <v>185</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -2111,15 +2112,15 @@
       </c>
       <c r="B4">
         <f>COUNTIFS('Selected keepers'!B:B,A4,'Selected keepers'!E:E,"x")</f>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="C4">
         <f>SUMIFS('Selected keepers'!J:J,'Selected keepers'!B:B,A4,'Selected keepers'!E:E,"x")</f>
-        <v>0</v>
+        <v>6162</v>
       </c>
       <c r="D4">
         <f>'Team salary worksheet'!$N$11-C4</f>
-        <v>6180</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -2128,15 +2129,15 @@
       </c>
       <c r="B5">
         <f>COUNTIFS('Selected keepers'!B:B,A5,'Selected keepers'!E:E,"x")</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="C5">
         <f>SUMIFS('Selected keepers'!J:J,'Selected keepers'!B:B,A5,'Selected keepers'!E:E,"x")</f>
-        <v>0</v>
+        <v>5995</v>
       </c>
       <c r="D5">
         <f>'Team salary worksheet'!$N$11-C5</f>
-        <v>6180</v>
+        <v>185</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -2145,15 +2146,15 @@
       </c>
       <c r="B6">
         <f>COUNTIFS('Selected keepers'!B:B,A6,'Selected keepers'!E:E,"x")</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C6">
         <f>SUMIFS('Selected keepers'!J:J,'Selected keepers'!B:B,A6,'Selected keepers'!E:E,"x")</f>
-        <v>0</v>
+        <v>3458</v>
       </c>
       <c r="D6">
         <f>'Team salary worksheet'!$N$11-C6</f>
-        <v>6180</v>
+        <v>2722</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -2162,15 +2163,15 @@
       </c>
       <c r="B7">
         <f>COUNTIFS('Selected keepers'!B:B,A7,'Selected keepers'!E:E,"x")</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="C7">
         <f>SUMIFS('Selected keepers'!J:J,'Selected keepers'!B:B,A7,'Selected keepers'!E:E,"x")</f>
-        <v>0</v>
+        <v>4250</v>
       </c>
       <c r="D7">
         <f>'Team salary worksheet'!$N$11-C7</f>
-        <v>6180</v>
+        <v>1930</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -2179,15 +2180,15 @@
       </c>
       <c r="B8">
         <f>COUNTIFS('Selected keepers'!B:B,A8,'Selected keepers'!E:E,"x")</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="C8">
         <f>SUMIFS('Selected keepers'!J:J,'Selected keepers'!B:B,A8,'Selected keepers'!E:E,"x")</f>
-        <v>0</v>
+        <v>5589</v>
       </c>
       <c r="D8">
         <f>'Team salary worksheet'!$N$11-C8</f>
-        <v>6180</v>
+        <v>591</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -2196,15 +2197,15 @@
       </c>
       <c r="B9">
         <f>COUNTIFS('Selected keepers'!B:B,A9,'Selected keepers'!E:E,"x")</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="C9">
         <f>SUMIFS('Selected keepers'!J:J,'Selected keepers'!B:B,A9,'Selected keepers'!E:E,"x")</f>
-        <v>0</v>
+        <v>5969</v>
       </c>
       <c r="D9">
         <f>'Team salary worksheet'!$N$11-C9</f>
-        <v>6180</v>
+        <v>211</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -2213,15 +2214,15 @@
       </c>
       <c r="B10">
         <f>COUNTIFS('Selected keepers'!B:B,A10,'Selected keepers'!E:E,"x")</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C10">
         <f>SUMIFS('Selected keepers'!J:J,'Selected keepers'!B:B,A10,'Selected keepers'!E:E,"x")</f>
-        <v>0</v>
+        <v>4119</v>
       </c>
       <c r="D10">
         <f>'Team salary worksheet'!$N$11-C10</f>
-        <v>6180</v>
+        <v>2061</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -2230,15 +2231,15 @@
       </c>
       <c r="B11">
         <f>COUNTIFS('Selected keepers'!B:B,A11,'Selected keepers'!E:E,"x")</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C11">
         <f>SUMIFS('Selected keepers'!J:J,'Selected keepers'!B:B,A11,'Selected keepers'!E:E,"x")</f>
-        <v>0</v>
+        <v>6104</v>
       </c>
       <c r="D11">
         <f>'Team salary worksheet'!$N$11-C11</f>
-        <v>6180</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -2258,7 +2259,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2389,7 +2390,9 @@
       <c r="D3" t="s">
         <v>171</v>
       </c>
-      <c r="E3" s="3"/>
+      <c r="E3" s="3" t="s">
+        <v>386</v>
+      </c>
       <c r="F3" t="s">
         <v>299</v>
       </c>
@@ -2437,6 +2440,9 @@
       <c r="D4" t="s">
         <v>171</v>
       </c>
+      <c r="E4" s="3" t="s">
+        <v>386</v>
+      </c>
       <c r="F4" t="s">
         <v>299</v>
       </c>
@@ -2540,6 +2546,9 @@
       <c r="D6" t="s">
         <v>317</v>
       </c>
+      <c r="E6" s="3" t="s">
+        <v>386</v>
+      </c>
       <c r="F6" t="s">
         <v>318</v>
       </c>
@@ -2652,6 +2661,9 @@
       <c r="D8" t="s">
         <v>317</v>
       </c>
+      <c r="E8" s="3" t="s">
+        <v>386</v>
+      </c>
       <c r="F8" t="s">
         <v>299</v>
       </c>
@@ -2764,7 +2776,9 @@
       <c r="D10" t="s">
         <v>182</v>
       </c>
-      <c r="E10" s="3"/>
+      <c r="E10" s="3" t="s">
+        <v>386</v>
+      </c>
       <c r="F10" t="s">
         <v>318</v>
       </c>
@@ -2877,6 +2891,9 @@
       <c r="D12" t="s">
         <v>319</v>
       </c>
+      <c r="E12" s="3" t="s">
+        <v>386</v>
+      </c>
       <c r="F12" t="s">
         <v>299</v>
       </c>
@@ -2933,6 +2950,9 @@
       <c r="D13" t="s">
         <v>322</v>
       </c>
+      <c r="E13" s="3" t="s">
+        <v>386</v>
+      </c>
       <c r="F13" t="s">
         <v>318</v>
       </c>
@@ -2989,6 +3009,9 @@
       <c r="D14" t="s">
         <v>174</v>
       </c>
+      <c r="E14" s="3" t="s">
+        <v>386</v>
+      </c>
       <c r="F14" t="s">
         <v>318</v>
       </c>
@@ -3045,6 +3068,9 @@
       <c r="D15" t="s">
         <v>179</v>
       </c>
+      <c r="E15" s="3" t="s">
+        <v>386</v>
+      </c>
       <c r="F15" t="s">
         <v>318</v>
       </c>
@@ -3101,6 +3127,9 @@
       <c r="D16" t="s">
         <v>185</v>
       </c>
+      <c r="E16" s="3" t="s">
+        <v>386</v>
+      </c>
       <c r="F16" t="s">
         <v>299</v>
       </c>
@@ -3157,6 +3186,9 @@
       <c r="D17" t="s">
         <v>185</v>
       </c>
+      <c r="E17" s="3" t="s">
+        <v>386</v>
+      </c>
       <c r="F17" t="s">
         <v>318</v>
       </c>
@@ -3493,6 +3525,9 @@
       <c r="D23" t="s">
         <v>185</v>
       </c>
+      <c r="E23" s="3" t="s">
+        <v>386</v>
+      </c>
       <c r="F23" t="s">
         <v>324</v>
       </c>
@@ -3820,7 +3855,9 @@
       <c r="D29" t="s">
         <v>174</v>
       </c>
-      <c r="E29" s="3"/>
+      <c r="E29" s="3" t="s">
+        <v>386</v>
+      </c>
       <c r="F29" t="s">
         <v>318</v>
       </c>
@@ -3924,6 +3961,9 @@
       <c r="D31" t="s">
         <v>182</v>
       </c>
+      <c r="E31" s="3" t="s">
+        <v>386</v>
+      </c>
       <c r="F31" t="s">
         <v>318</v>
       </c>
@@ -3980,6 +4020,9 @@
       <c r="D32" t="s">
         <v>171</v>
       </c>
+      <c r="E32" s="3" t="s">
+        <v>386</v>
+      </c>
       <c r="F32" t="s">
         <v>299</v>
       </c>
@@ -4027,6 +4070,7 @@
       <c r="D33" t="s">
         <v>182</v>
       </c>
+      <c r="E33" s="3"/>
       <c r="F33" t="s">
         <v>299</v>
       </c>
@@ -4083,6 +4127,9 @@
       <c r="D34" t="s">
         <v>179</v>
       </c>
+      <c r="E34" s="3" t="s">
+        <v>386</v>
+      </c>
       <c r="F34" t="s">
         <v>299</v>
       </c>
@@ -4139,6 +4186,9 @@
       <c r="D35" t="s">
         <v>171</v>
       </c>
+      <c r="E35" s="3" t="s">
+        <v>386</v>
+      </c>
       <c r="F35" t="s">
         <v>299</v>
       </c>
@@ -4186,6 +4236,9 @@
       <c r="D36" t="s">
         <v>179</v>
       </c>
+      <c r="E36" s="3" t="s">
+        <v>386</v>
+      </c>
       <c r="F36" t="s">
         <v>299</v>
       </c>
@@ -4354,6 +4407,9 @@
       <c r="D39" t="s">
         <v>174</v>
       </c>
+      <c r="E39" s="3" t="s">
+        <v>386</v>
+      </c>
       <c r="F39" t="s">
         <v>318</v>
       </c>
@@ -4410,6 +4466,9 @@
       <c r="D40" t="s">
         <v>322</v>
       </c>
+      <c r="E40" s="3" t="s">
+        <v>386</v>
+      </c>
       <c r="F40" t="s">
         <v>299</v>
       </c>
@@ -4466,6 +4525,9 @@
       <c r="D41" t="s">
         <v>185</v>
       </c>
+      <c r="E41" s="3" t="s">
+        <v>386</v>
+      </c>
       <c r="F41" t="s">
         <v>299</v>
       </c>
@@ -4849,6 +4911,9 @@
       <c r="D48" t="s">
         <v>185</v>
       </c>
+      <c r="E48" s="3" t="s">
+        <v>386</v>
+      </c>
       <c r="F48" t="s">
         <v>324</v>
       </c>
@@ -4905,6 +4970,9 @@
       <c r="D49" t="s">
         <v>322</v>
       </c>
+      <c r="E49" s="3" t="s">
+        <v>386</v>
+      </c>
       <c r="F49" t="s">
         <v>324</v>
       </c>
@@ -5503,6 +5571,9 @@
       <c r="D60" t="s">
         <v>182</v>
       </c>
+      <c r="E60" s="3" t="s">
+        <v>386</v>
+      </c>
       <c r="F60" t="s">
         <v>299</v>
       </c>
@@ -5559,6 +5630,9 @@
       <c r="D61" t="s">
         <v>185</v>
       </c>
+      <c r="E61" s="3" t="s">
+        <v>386</v>
+      </c>
       <c r="F61" t="s">
         <v>318</v>
       </c>
@@ -5671,6 +5745,9 @@
       <c r="D63" t="s">
         <v>174</v>
       </c>
+      <c r="E63" s="3" t="s">
+        <v>386</v>
+      </c>
       <c r="F63" t="s">
         <v>318</v>
       </c>
@@ -5727,6 +5804,9 @@
       <c r="D64" t="s">
         <v>319</v>
       </c>
+      <c r="E64" s="3" t="s">
+        <v>386</v>
+      </c>
       <c r="F64" t="s">
         <v>299</v>
       </c>
@@ -5783,6 +5863,9 @@
       <c r="D65" t="s">
         <v>174</v>
       </c>
+      <c r="E65" s="3" t="s">
+        <v>386</v>
+      </c>
       <c r="F65" t="s">
         <v>318</v>
       </c>
@@ -5839,6 +5922,9 @@
       <c r="D66" t="s">
         <v>179</v>
       </c>
+      <c r="E66" s="3" t="s">
+        <v>386</v>
+      </c>
       <c r="F66" t="s">
         <v>299</v>
       </c>
@@ -5951,6 +6037,9 @@
       <c r="D68" t="s">
         <v>182</v>
       </c>
+      <c r="E68" s="3" t="s">
+        <v>386</v>
+      </c>
       <c r="F68" t="s">
         <v>299</v>
       </c>
@@ -6110,6 +6199,9 @@
       <c r="D71" t="s">
         <v>174</v>
       </c>
+      <c r="E71" s="3" t="s">
+        <v>386</v>
+      </c>
       <c r="F71" t="s">
         <v>299</v>
       </c>
@@ -6166,6 +6258,9 @@
       <c r="D72" t="s">
         <v>179</v>
       </c>
+      <c r="E72" s="3" t="s">
+        <v>386</v>
+      </c>
       <c r="F72" t="s">
         <v>318</v>
       </c>
@@ -6222,6 +6317,9 @@
       <c r="D73" t="s">
         <v>185</v>
       </c>
+      <c r="E73" s="3" t="s">
+        <v>386</v>
+      </c>
       <c r="F73" t="s">
         <v>318</v>
       </c>
@@ -6278,6 +6376,9 @@
       <c r="D74" t="s">
         <v>322</v>
       </c>
+      <c r="E74" s="3" t="s">
+        <v>386</v>
+      </c>
       <c r="F74" t="s">
         <v>324</v>
       </c>
@@ -6334,6 +6435,9 @@
       <c r="D75" t="s">
         <v>185</v>
       </c>
+      <c r="E75" s="3" t="s">
+        <v>386</v>
+      </c>
       <c r="F75" t="s">
         <v>318</v>
       </c>
@@ -6390,6 +6494,9 @@
       <c r="D76" t="s">
         <v>185</v>
       </c>
+      <c r="E76" s="3" t="s">
+        <v>386</v>
+      </c>
       <c r="F76" t="s">
         <v>299</v>
       </c>
@@ -6558,6 +6665,9 @@
       <c r="D79" t="s">
         <v>171</v>
       </c>
+      <c r="E79" s="3" t="s">
+        <v>386</v>
+      </c>
       <c r="F79" t="s">
         <v>318</v>
       </c>
@@ -6605,6 +6715,9 @@
       <c r="D80" t="s">
         <v>182</v>
       </c>
+      <c r="E80" s="3" t="s">
+        <v>386</v>
+      </c>
       <c r="F80" t="s">
         <v>318</v>
       </c>
@@ -6661,6 +6774,9 @@
       <c r="D81" t="s">
         <v>317</v>
       </c>
+      <c r="E81" s="3" t="s">
+        <v>386</v>
+      </c>
       <c r="F81" t="s">
         <v>324</v>
       </c>
@@ -6961,6 +7077,9 @@
       <c r="D87" t="s">
         <v>182</v>
       </c>
+      <c r="E87" s="3" t="s">
+        <v>386</v>
+      </c>
       <c r="F87" t="s">
         <v>318</v>
       </c>
@@ -7017,6 +7136,9 @@
       <c r="D88" t="s">
         <v>174</v>
       </c>
+      <c r="E88" s="3" t="s">
+        <v>386</v>
+      </c>
       <c r="F88" t="s">
         <v>318</v>
       </c>
@@ -7129,6 +7251,9 @@
       <c r="D90" t="s">
         <v>179</v>
       </c>
+      <c r="E90" s="3" t="s">
+        <v>386</v>
+      </c>
       <c r="F90" t="s">
         <v>318</v>
       </c>
@@ -7185,6 +7310,9 @@
       <c r="D91" t="s">
         <v>171</v>
       </c>
+      <c r="E91" s="3" t="s">
+        <v>386</v>
+      </c>
       <c r="F91" t="s">
         <v>318</v>
       </c>
@@ -7232,6 +7360,9 @@
       <c r="D92" t="s">
         <v>185</v>
       </c>
+      <c r="E92" s="3" t="s">
+        <v>386</v>
+      </c>
       <c r="F92" t="s">
         <v>318</v>
       </c>
@@ -7456,6 +7587,9 @@
       <c r="D96" t="s">
         <v>322</v>
       </c>
+      <c r="E96" s="3" t="s">
+        <v>386</v>
+      </c>
       <c r="F96" t="s">
         <v>299</v>
       </c>
@@ -7512,6 +7646,9 @@
       <c r="D97" t="s">
         <v>185</v>
       </c>
+      <c r="E97" s="3" t="s">
+        <v>386</v>
+      </c>
       <c r="F97" t="s">
         <v>299</v>
       </c>
@@ -8541,6 +8678,9 @@
       <c r="D116" t="s">
         <v>182</v>
       </c>
+      <c r="E116" s="3" t="s">
+        <v>386</v>
+      </c>
       <c r="F116" t="s">
         <v>318</v>
       </c>
@@ -9045,6 +9185,9 @@
       <c r="D125" t="s">
         <v>182</v>
       </c>
+      <c r="E125" s="3" t="s">
+        <v>386</v>
+      </c>
       <c r="F125" t="s">
         <v>299</v>
       </c>
@@ -9157,6 +9300,9 @@
       <c r="D127" t="s">
         <v>182</v>
       </c>
+      <c r="E127" s="3" t="s">
+        <v>386</v>
+      </c>
       <c r="F127" t="s">
         <v>318</v>
       </c>
@@ -9316,6 +9462,9 @@
       <c r="D130" t="s">
         <v>171</v>
       </c>
+      <c r="E130" s="3" t="s">
+        <v>386</v>
+      </c>
       <c r="F130" t="s">
         <v>318</v>
       </c>
@@ -9475,6 +9624,9 @@
       <c r="D133" t="s">
         <v>174</v>
       </c>
+      <c r="E133" s="3" t="s">
+        <v>386</v>
+      </c>
       <c r="F133" t="s">
         <v>299</v>
       </c>
@@ -9634,6 +9786,9 @@
       <c r="D136" t="s">
         <v>322</v>
       </c>
+      <c r="E136" s="3" t="s">
+        <v>386</v>
+      </c>
       <c r="F136" t="s">
         <v>318</v>
       </c>
@@ -10046,6 +10201,9 @@
       <c r="D144" t="s">
         <v>174</v>
       </c>
+      <c r="E144" s="3" t="s">
+        <v>386</v>
+      </c>
       <c r="F144" t="s">
         <v>299</v>
       </c>
@@ -10158,6 +10316,9 @@
       <c r="D146" t="s">
         <v>182</v>
       </c>
+      <c r="E146" s="3" t="s">
+        <v>386</v>
+      </c>
       <c r="F146" t="s">
         <v>299</v>
       </c>
@@ -10214,6 +10375,9 @@
       <c r="D147" t="s">
         <v>174</v>
       </c>
+      <c r="E147" s="3" t="s">
+        <v>386</v>
+      </c>
       <c r="F147" t="s">
         <v>299</v>
       </c>
@@ -10326,6 +10490,9 @@
       <c r="D149" t="s">
         <v>182</v>
       </c>
+      <c r="E149" s="3" t="s">
+        <v>386</v>
+      </c>
       <c r="F149" t="s">
         <v>299</v>
       </c>
@@ -10550,6 +10717,9 @@
       <c r="D153" t="s">
         <v>319</v>
       </c>
+      <c r="E153" s="3" t="s">
+        <v>386</v>
+      </c>
       <c r="F153" t="s">
         <v>324</v>
       </c>
@@ -10718,6 +10888,9 @@
       <c r="D156" t="s">
         <v>322</v>
       </c>
+      <c r="E156" s="3" t="s">
+        <v>386</v>
+      </c>
       <c r="F156" t="s">
         <v>299</v>
       </c>
@@ -10830,6 +11003,9 @@
       <c r="D158" t="s">
         <v>171</v>
       </c>
+      <c r="E158" s="3" t="s">
+        <v>386</v>
+      </c>
       <c r="F158" t="s">
         <v>318</v>
       </c>
@@ -11540,6 +11716,9 @@
       <c r="D171" t="s">
         <v>174</v>
       </c>
+      <c r="E171" s="3" t="s">
+        <v>386</v>
+      </c>
       <c r="F171" t="s">
         <v>299</v>
       </c>
@@ -11596,6 +11775,9 @@
       <c r="D172" t="s">
         <v>174</v>
       </c>
+      <c r="E172" s="3" t="s">
+        <v>386</v>
+      </c>
       <c r="F172" t="s">
         <v>318</v>
       </c>
@@ -11652,6 +11834,9 @@
       <c r="D173" t="s">
         <v>174</v>
       </c>
+      <c r="E173" s="3" t="s">
+        <v>386</v>
+      </c>
       <c r="F173" t="s">
         <v>299</v>
       </c>
@@ -11820,6 +12005,9 @@
       <c r="D176" t="s">
         <v>171</v>
       </c>
+      <c r="E176" s="3" t="s">
+        <v>386</v>
+      </c>
       <c r="F176" t="s">
         <v>318</v>
       </c>
@@ -11914,6 +12102,9 @@
       <c r="D178" t="s">
         <v>174</v>
       </c>
+      <c r="E178" s="3" t="s">
+        <v>386</v>
+      </c>
       <c r="F178" t="s">
         <v>318</v>
       </c>
@@ -12082,6 +12273,9 @@
       <c r="D181" t="s">
         <v>182</v>
       </c>
+      <c r="E181" s="3" t="s">
+        <v>386</v>
+      </c>
       <c r="F181" t="s">
         <v>324</v>
       </c>
@@ -12138,6 +12332,9 @@
       <c r="D182" t="s">
         <v>179</v>
       </c>
+      <c r="E182" s="3" t="s">
+        <v>386</v>
+      </c>
       <c r="F182" t="s">
         <v>324</v>
       </c>
@@ -12241,6 +12438,9 @@
       <c r="D184" t="s">
         <v>317</v>
       </c>
+      <c r="E184" s="3" t="s">
+        <v>386</v>
+      </c>
       <c r="F184" t="s">
         <v>299</v>
       </c>
@@ -12297,6 +12497,9 @@
       <c r="D185" t="s">
         <v>317</v>
       </c>
+      <c r="E185" s="3" t="s">
+        <v>386</v>
+      </c>
       <c r="F185" t="s">
         <v>324</v>
       </c>
@@ -12353,6 +12556,9 @@
       <c r="D186" t="s">
         <v>185</v>
       </c>
+      <c r="E186" s="3" t="s">
+        <v>386</v>
+      </c>
       <c r="F186" t="s">
         <v>324</v>
       </c>
@@ -12465,6 +12671,9 @@
       <c r="D188" t="s">
         <v>322</v>
       </c>
+      <c r="E188" s="3" t="s">
+        <v>386</v>
+      </c>
       <c r="F188" t="s">
         <v>324</v>
       </c>
@@ -13175,6 +13384,9 @@
       <c r="D201" t="s">
         <v>174</v>
       </c>
+      <c r="E201" t="s">
+        <v>386</v>
+      </c>
       <c r="F201" t="s">
         <v>318</v>
       </c>
@@ -13287,6 +13499,9 @@
       <c r="D203" t="s">
         <v>171</v>
       </c>
+      <c r="E203" t="s">
+        <v>386</v>
+      </c>
       <c r="F203" t="s">
         <v>299</v>
       </c>
@@ -13390,6 +13605,9 @@
       <c r="D205" t="s">
         <v>174</v>
       </c>
+      <c r="E205" t="s">
+        <v>386</v>
+      </c>
       <c r="F205" t="s">
         <v>324</v>
       </c>
@@ -13558,6 +13776,9 @@
       <c r="D208" t="s">
         <v>179</v>
       </c>
+      <c r="E208" t="s">
+        <v>386</v>
+      </c>
       <c r="F208" t="s">
         <v>299</v>
       </c>
@@ -13614,6 +13835,9 @@
       <c r="D209" t="s">
         <v>174</v>
       </c>
+      <c r="E209" t="s">
+        <v>386</v>
+      </c>
       <c r="F209" t="s">
         <v>318</v>
       </c>
@@ -13670,6 +13894,9 @@
       <c r="D210" t="s">
         <v>319</v>
       </c>
+      <c r="E210" t="s">
+        <v>386</v>
+      </c>
       <c r="F210" t="s">
         <v>299</v>
       </c>
@@ -13726,6 +13953,9 @@
       <c r="D211" t="s">
         <v>171</v>
       </c>
+      <c r="E211" t="s">
+        <v>386</v>
+      </c>
       <c r="F211" t="s">
         <v>299</v>
       </c>
@@ -13773,6 +14003,9 @@
       <c r="D212" t="s">
         <v>317</v>
       </c>
+      <c r="E212" t="s">
+        <v>386</v>
+      </c>
       <c r="F212" t="s">
         <v>324</v>
       </c>
@@ -13829,6 +14062,9 @@
       <c r="D213" t="s">
         <v>319</v>
       </c>
+      <c r="E213" t="s">
+        <v>386</v>
+      </c>
       <c r="F213" t="s">
         <v>299</v>
       </c>
@@ -13885,6 +14121,9 @@
       <c r="D214" t="s">
         <v>179</v>
       </c>
+      <c r="E214" t="s">
+        <v>386</v>
+      </c>
       <c r="F214" t="s">
         <v>299</v>
       </c>
@@ -13941,6 +14180,9 @@
       <c r="D215" t="s">
         <v>182</v>
       </c>
+      <c r="E215" t="s">
+        <v>386</v>
+      </c>
       <c r="F215" t="s">
         <v>299</v>
       </c>
@@ -14221,6 +14463,9 @@
       <c r="D220" t="s">
         <v>171</v>
       </c>
+      <c r="E220" t="s">
+        <v>386</v>
+      </c>
       <c r="F220" t="s">
         <v>299</v>
       </c>
@@ -14427,6 +14672,9 @@
       <c r="D224" t="s">
         <v>185</v>
       </c>
+      <c r="E224" t="s">
+        <v>386</v>
+      </c>
       <c r="F224" t="s">
         <v>324</v>
       </c>
@@ -14586,6 +14834,9 @@
       <c r="D227" t="s">
         <v>185</v>
       </c>
+      <c r="E227" t="s">
+        <v>386</v>
+      </c>
       <c r="F227" t="s">
         <v>318</v>
       </c>
@@ -14801,6 +15052,9 @@
       <c r="D231" t="s">
         <v>171</v>
       </c>
+      <c r="E231" s="3" t="s">
+        <v>386</v>
+      </c>
       <c r="F231" t="s">
         <v>318</v>
       </c>
@@ -14904,6 +15158,9 @@
       <c r="D233" t="s">
         <v>317</v>
       </c>
+      <c r="E233" s="3" t="s">
+        <v>386</v>
+      </c>
       <c r="F233" t="s">
         <v>324</v>
       </c>
@@ -15016,6 +15273,9 @@
       <c r="D235" t="s">
         <v>185</v>
       </c>
+      <c r="E235" s="3" t="s">
+        <v>386</v>
+      </c>
       <c r="F235" t="s">
         <v>318</v>
       </c>
@@ -15072,6 +15332,9 @@
       <c r="D236" t="s">
         <v>185</v>
       </c>
+      <c r="E236" s="3" t="s">
+        <v>386</v>
+      </c>
       <c r="F236" t="s">
         <v>318</v>
       </c>
@@ -15128,6 +15391,9 @@
       <c r="D237" t="s">
         <v>174</v>
       </c>
+      <c r="E237" s="3" t="s">
+        <v>386</v>
+      </c>
       <c r="F237" t="s">
         <v>318</v>
       </c>
@@ -15464,6 +15730,9 @@
       <c r="D243" t="s">
         <v>185</v>
       </c>
+      <c r="E243" s="3" t="s">
+        <v>386</v>
+      </c>
       <c r="F243" t="s">
         <v>318</v>
       </c>
@@ -15576,6 +15845,9 @@
       <c r="D245" t="s">
         <v>185</v>
       </c>
+      <c r="E245" s="3" t="s">
+        <v>386</v>
+      </c>
       <c r="F245" t="s">
         <v>299</v>
       </c>
@@ -15744,6 +16016,9 @@
       <c r="D248" t="s">
         <v>185</v>
       </c>
+      <c r="E248" s="3" t="s">
+        <v>386</v>
+      </c>
       <c r="F248" t="s">
         <v>324</v>
       </c>
@@ -16295,6 +16570,9 @@
       <c r="D258" t="s">
         <v>319</v>
       </c>
+      <c r="E258" s="3" t="s">
+        <v>386</v>
+      </c>
       <c r="F258" t="s">
         <v>318</v>
       </c>
@@ -16351,6 +16629,9 @@
       <c r="D259" t="s">
         <v>171</v>
       </c>
+      <c r="E259" s="3" t="s">
+        <v>386</v>
+      </c>
       <c r="F259" t="s">
         <v>299</v>
       </c>
@@ -16398,6 +16679,9 @@
       <c r="D260" t="s">
         <v>171</v>
       </c>
+      <c r="E260" s="3" t="s">
+        <v>386</v>
+      </c>
       <c r="F260" t="s">
         <v>299</v>
       </c>
@@ -16613,6 +16897,9 @@
       <c r="D264" t="s">
         <v>174</v>
       </c>
+      <c r="E264" s="3" t="s">
+        <v>386</v>
+      </c>
       <c r="F264" t="s">
         <v>299</v>
       </c>
@@ -16772,6 +17059,9 @@
       <c r="D267" t="s">
         <v>182</v>
       </c>
+      <c r="E267" s="3" t="s">
+        <v>386</v>
+      </c>
       <c r="F267" t="s">
         <v>299</v>
       </c>
@@ -16828,6 +17118,9 @@
       <c r="D268" t="s">
         <v>174</v>
       </c>
+      <c r="E268" s="3" t="s">
+        <v>386</v>
+      </c>
       <c r="F268" t="s">
         <v>299</v>
       </c>
@@ -16884,6 +17177,9 @@
       <c r="D269" t="s">
         <v>322</v>
       </c>
+      <c r="E269" s="3" t="s">
+        <v>386</v>
+      </c>
       <c r="F269" t="s">
         <v>318</v>
       </c>
@@ -16940,6 +17236,9 @@
       <c r="D270" t="s">
         <v>185</v>
       </c>
+      <c r="E270" s="3" t="s">
+        <v>386</v>
+      </c>
       <c r="F270" t="s">
         <v>318</v>
       </c>
@@ -17043,6 +17342,9 @@
       <c r="D272" t="s">
         <v>185</v>
       </c>
+      <c r="E272" s="3" t="s">
+        <v>386</v>
+      </c>
       <c r="F272" t="s">
         <v>318</v>
       </c>
@@ -17154,6 +17456,9 @@
       </c>
       <c r="D274" t="s">
         <v>185</v>
+      </c>
+      <c r="E274" s="3" t="s">
+        <v>386</v>
       </c>
       <c r="F274" t="s">
         <v>318</v>
@@ -17726,7 +18031,7 @@
   </sheetPr>
   <dimension ref="A2:Q40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:G2"/>
     </sheetView>
   </sheetViews>

</xml_diff>